<commit_message>
just commited everything, small changes
</commit_message>
<xml_diff>
--- a/data/db_substance.xlsx
+++ b/data/db_substance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hkw\uni\Vertiefung_Gröschel\R\ggpolymer\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hkw\uni\Masterarbeit\R\ggpolymer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAB682F-4503-499F-AF8A-7F8283DEB90C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED820CF-C227-4517-BA7B-72D9D3703E20}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9036" yWindow="5436" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>substance</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>PEO2k</t>
+  </si>
+  <si>
+    <t>HMTETA</t>
+  </si>
+  <si>
+    <t>HW45-PtBMA</t>
+  </si>
+  <si>
+    <t>HW49-PtBMA-END</t>
+  </si>
+  <si>
+    <t>HW55-PtBMA-Prod</t>
   </si>
 </sst>
 </file>
@@ -408,14 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" customWidth="1"/>
@@ -597,6 +610,65 @@
         <v>9</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>230.39</v>
+      </c>
+      <c r="D12">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>8156</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>8500</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>8674</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>